<commit_message>
changed data representation and results bigger fonts in diagrams
</commit_message>
<xml_diff>
--- a/data/4.5.20_log_outputs/Data.xlsx
+++ b/data/4.5.20_log_outputs/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\uni\dissertation\data\4.5.20_log_outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\diss data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9713F009-89D0-4D86-8F73-6E18A538F472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09451E6F-422E-4B51-ACAD-F53EA86A355C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="1035" windowWidth="21600" windowHeight="11505" xr2:uid="{7DEA8850-E494-4A9B-99A5-9AE54C86D9B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{7DEA8850-E494-4A9B-99A5-9AE54C86D9B5}"/>
   </bookViews>
   <sheets>
     <sheet name="105321 (raw latency)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
   <si>
     <t>UTC</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>11.13.52.249</t>
+  </si>
+  <si>
+    <t>Expected Frame Rate</t>
+  </si>
+  <si>
+    <t>Used Bandwidth</t>
   </si>
 </sst>
 </file>
@@ -1512,6 +1518,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="699511216"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1635,11 +1642,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Transmission latency with manually</a:t>
+              <a:t>Transmission latency with manual</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> specified step</a:t>
+              <a:t> expected FPS</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2139,19 +2146,19 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'111207 (instability)'!$H$1</c:f>
+              <c:f>'111207 (instability)'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Step</c:v>
+                  <c:v>Expected Frame Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2162,186 +2169,186 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'111207 (instability)'!$H$2:$H$60</c:f>
+              <c:f>'111207 (instability)'!$K$2:$K$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="59"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2350,6 +2357,225 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-091B-4DDB-AD8C-194C5D99F683}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'111207 (instability)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'111207 (instability)'!$C$2:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>14.720314033366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.8267716535433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.8267716535433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.7326150832517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.670910871694399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.7878192534381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.757605495583899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9164208456243896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.8939096267190596</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8495575221238898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9685039370078701</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.9115913555992101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.8493150684931496</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.8508341511285602</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.8431372549019596</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.8939096267190596</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.8829891838741402</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.7531831537708</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.6899224806201492</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.8740157480314998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.9019607843137303</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.8425196850393704</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.9115913555992101</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.8923679060665402</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11.7531831537708</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.8425196850393704</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EAD5-419F-9846-833845C7B349}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2361,10 +2587,47 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="20000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="20000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="20000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="20000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="708932632"/>
-        <c:axId val="708931648"/>
+        <c:axId val="454690424"/>
+        <c:axId val="454684520"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="708585256"/>
@@ -2593,10 +2856,10 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="708931648"/>
+        <c:axId val="454684520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -2621,7 +2884,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Step</a:t>
+                  <a:t>Frame Rate</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2686,12 +2949,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708932632"/>
+        <c:crossAx val="454690424"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="708932632"/>
+        <c:axId val="454690424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2700,7 +2963,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="708931648"/>
+        <c:crossAx val="454684520"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2828,7 +3092,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> of cloud based server with manually specified step</a:t>
+              <a:t> of cloud based server with manual expected FPS</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2878,7 +3142,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mbps</c:v>
+                  <c:v>Used Bandwidth</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3109,19 +3373,19 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'111207 (instability)'!$H$1</c:f>
+              <c:f>'111207 (instability)'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Step</c:v>
+                  <c:v>Expected Frame Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3132,186 +3396,186 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'111207 (instability)'!$H$2:$H$60</c:f>
+              <c:f>'111207 (instability)'!$K$2:$K$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="59"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.8</c:v>
+                  <c:v>5.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3320,6 +3584,225 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F768-49B6-91B3-5E056F958DA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'111207 (instability)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'111207 (instability)'!$C$2:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>14.720314033366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.8267716535433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.8267716535433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.7326150832517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.670910871694399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.7878192534381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.757605495583899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9164208456243896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.8939096267190596</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8495575221238898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9685039370078701</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.9115913555992101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.8493150684931496</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.8508341511285602</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.8431372549019596</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.8939096267190596</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9527559055118102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.8829891838741402</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.7531831537708</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.6899224806201492</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.9055118110236204</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.8740157480314998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.9019607843137303</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.8425196850393704</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.9115913555992101</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.9212598425196896</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9370078740157499</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.8923679060665402</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11.7531831537708</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.8425196850393704</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.8897637795275601</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0588-4A64-A689-81775764B04D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3331,6 +3814,43 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="20000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="20000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="20000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="20000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="709645136"/>
@@ -3483,7 +4003,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Bandwidth</a:t>
+                  <a:t>Bandwidth (Mbps)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3556,7 +4076,7 @@
         <c:axId val="709642184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -3581,7 +4101,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Step</a:t>
+                  <a:t>Frame Rate</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3661,6 +4181,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="709642184"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5462,16 +5983,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5498,16 +6019,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5834,7 +6355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D81E87A-6355-424D-896B-0F0B2EE0BA6A}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
@@ -7826,15 +8347,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96F3BBE-38A7-40DE-A68C-8E25010BFE48}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7845,7 +8366,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -7865,8 +8386,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -7897,8 +8421,12 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>(1-H2)*30</f>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -7929,8 +8457,12 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f t="shared" ref="K3:K60" si="0">(1-H3)*30</f>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -7961,8 +8493,12 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -7993,8 +8529,12 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -8025,8 +8565,12 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -8057,8 +8601,12 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -8089,8 +8637,12 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -8121,8 +8673,12 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -8153,8 +8709,12 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -8185,8 +8745,12 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -8217,8 +8781,12 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -8249,8 +8817,12 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -8281,8 +8853,12 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -8313,8 +8889,12 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -8345,8 +8925,12 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -8377,8 +8961,12 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -8409,8 +8997,12 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -8441,8 +9033,12 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -8473,8 +9069,12 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -8505,8 +9105,12 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -8537,8 +9141,12 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -8569,8 +9177,12 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -8601,8 +9213,12 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -8633,8 +9249,12 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -8665,8 +9285,12 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -8697,8 +9321,12 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -8729,8 +9357,12 @@
       <c r="J28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -8761,8 +9393,12 @@
       <c r="J29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -8793,8 +9429,12 @@
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -8825,8 +9465,12 @@
       <c r="J31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -8857,8 +9501,12 @@
       <c r="J32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -8889,8 +9537,12 @@
       <c r="J33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -8921,8 +9573,12 @@
       <c r="J34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -8953,8 +9609,12 @@
       <c r="J35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -8985,8 +9645,12 @@
       <c r="J36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -9017,8 +9681,12 @@
       <c r="J37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>102</v>
       </c>
@@ -9049,8 +9717,12 @@
       <c r="J38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -9081,8 +9753,12 @@
       <c r="J39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -9113,8 +9789,12 @@
       <c r="J40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -9145,8 +9825,12 @@
       <c r="J41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -9177,8 +9861,12 @@
       <c r="J42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>107</v>
       </c>
@@ -9209,8 +9897,12 @@
       <c r="J43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>108</v>
       </c>
@@ -9241,8 +9933,12 @@
       <c r="J44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -9273,8 +9969,12 @@
       <c r="J45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -9305,8 +10005,12 @@
       <c r="J46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999982</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>111</v>
       </c>
@@ -9337,8 +10041,12 @@
       <c r="J47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -9369,8 +10077,12 @@
       <c r="J48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -9401,8 +10113,12 @@
       <c r="J49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -9433,8 +10149,12 @@
       <c r="J50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>115</v>
       </c>
@@ -9465,8 +10185,12 @@
       <c r="J51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>116</v>
       </c>
@@ -9497,8 +10221,12 @@
       <c r="J52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -9529,8 +10257,12 @@
       <c r="J53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>118</v>
       </c>
@@ -9561,8 +10293,12 @@
       <c r="J54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -9593,8 +10329,12 @@
       <c r="J55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -9625,8 +10365,12 @@
       <c r="J56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -9657,8 +10401,12 @@
       <c r="J57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -9689,8 +10437,12 @@
       <c r="J58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>123</v>
       </c>
@@ -9721,8 +10473,12 @@
       <c r="J59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -9752,6 +10508,10 @@
       </c>
       <c r="J60">
         <v>0</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>